<commit_message>
Exercícios SCRIPT - DML - DQL
</commit_message>
<xml_diff>
--- a/exercicios/1.1-exercicio-pessoas/Modelagem/Exercicio1.1-pessoas-FÍSICO.xlsx
+++ b/exercicios/1.1-exercicio-pessoas/Modelagem/Exercicio1.1-pessoas-FÍSICO.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/480d5ffb018c6fc9/Documentos/SENAI/Banco-de-Dados/exercicios/1.1-exercicio-pessoas/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/480d5ffb018c6fc9/Documentos/SENAI/Banco-de-Dados/exercicios/1.1-exercicio-pessoas/Modelagem/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="157" documentId="11_AD4D361C20488DEA4E38A0CD341D69CE5ADEDD9F" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2DEA0C06-75BD-4E8E-AD6A-62BF8AC78432}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2250" yWindow="2250" windowWidth="15375" windowHeight="7875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Plan1" sheetId="1" r:id="rId1"/>
@@ -670,7 +670,7 @@
   <dimension ref="A1:Q7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N15" sqref="N15"/>
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>